<commit_message>
Visualización de todos los datos
</commit_message>
<xml_diff>
--- a/Raw Data/Sujetos Equipo Beat.xlsx
+++ b/Raw Data/Sujetos Equipo Beat.xlsx
@@ -1,24 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos de trabajo\Electros\Github electro\Raw Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1CF640-5D10-4E1E-A363-E124456D56F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sujetos" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="S1A1" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="S2A1" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="S3A1" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="S4A1" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="S5A2" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="S6A2" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="S7A2" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="S8A2" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="S9A3" sheetId="10" r:id="rId13"/>
-    <sheet state="visible" name="S10A3" sheetId="11" r:id="rId14"/>
-    <sheet state="visible" name="S11A3" sheetId="12" r:id="rId15"/>
-    <sheet state="visible" name="S12A3" sheetId="13" r:id="rId16"/>
+    <sheet name="Sujetos" sheetId="1" r:id="rId1"/>
+    <sheet name="S1A1" sheetId="2" r:id="rId2"/>
+    <sheet name="S2A1" sheetId="3" r:id="rId3"/>
+    <sheet name="S3A1" sheetId="4" r:id="rId4"/>
+    <sheet name="S4A1" sheetId="5" r:id="rId5"/>
+    <sheet name="S5A2" sheetId="6" r:id="rId6"/>
+    <sheet name="S6A2" sheetId="7" r:id="rId7"/>
+    <sheet name="S7A2" sheetId="8" r:id="rId8"/>
+    <sheet name="S8A2" sheetId="9" r:id="rId9"/>
+    <sheet name="S9A3" sheetId="10" r:id="rId10"/>
+    <sheet name="S10A3" sheetId="11" r:id="rId11"/>
+    <sheet name="S11A3" sheetId="12" r:id="rId12"/>
+    <sheet name="S12A3" sheetId="13" r:id="rId13"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -145,28 +167,33 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font/>
-    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Inconsolata"/>
     </font>
@@ -176,7 +203,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -210,7 +237,13 @@
     </fill>
   </fills>
   <borders count="4">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -224,19 +257,23 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -246,143 +283,73 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -572,143 +539,141 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+      <c r="C2" s="18"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="C7" s="18"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="s">
+      <c r="C8" s="18"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="s">
+      <c r="C9" s="18"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
+      <c r="C10" s="18"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="8" t="s">
+      <c r="C11" s="18"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
+      <c r="C12" s="18"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -717,805 +682,828 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35:H36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.03333333333333333</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.11666666666666667</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="12">
         <f>(48)*256</f>
         <v>12288</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+48)*256</f>
         <v>43008</v>
       </c>
-      <c r="F2" s="14">
-        <f t="shared" ref="F2:F3" si="1">((C2+B2)/2)-B$12</f>
-        <v>0.05416666667</v>
-      </c>
-      <c r="G2" s="14">
-        <f t="shared" ref="G2:G3" si="2">((C2+B2)/2)+B$12</f>
-        <v>0.09583333333</v>
-      </c>
-      <c r="H2" s="21">
-        <v>78.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+      <c r="F2" s="10">
+        <f t="shared" ref="F2:F3" si="0">((C2+B2)/2)-B$12</f>
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" ref="G2:G3" si="1">((C2+B2)/2)+B$12</f>
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="H2" s="11">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.13055555555555556</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="10">
         <v>0.39791666666666664</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <f>((3*60)+8)*256</f>
         <v>48128</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((9*60)+33)*256</f>
         <v>146688</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="10">
+        <f t="shared" si="0"/>
+        <v>0.24340277777777777</v>
+      </c>
+      <c r="G3" s="10">
         <f t="shared" si="1"/>
-        <v>0.2434027778</v>
-      </c>
-      <c r="G3" s="14">
-        <f t="shared" si="2"/>
-        <v>0.2850694444</v>
-      </c>
-      <c r="H3" s="15">
+        <v>0.28506944444444443</v>
+      </c>
+      <c r="H3" s="11">
         <f>((5*60)+50)</f>
         <v>350</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
-        <v>0.4076388888888889</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="10">
+        <v>0.40763888888888888</v>
+      </c>
+      <c r="C4" s="10">
         <v>0.44930555555555557</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <f>((9*60)+47)*256</f>
         <v>150272</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((10*60)+47)*256</f>
         <v>165632</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
-        <v>0.4534722222222222</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.4951388888888889</v>
-      </c>
-      <c r="D5" s="16">
+      <c r="B5" s="10">
+        <v>0.45347222222222222</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.49513888888888891</v>
+      </c>
+      <c r="D5" s="12">
         <f>((10*60)+53)*256</f>
         <v>167168</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((11*60)+53)*256</f>
         <v>182528</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="10">
         <f>((C5+B5)/2)-B$12</f>
-        <v>0.4534722222</v>
-      </c>
-      <c r="G5" s="14">
+        <v>0.45347222222222222</v>
+      </c>
+      <c r="G5" s="10">
         <f>((C5+B5)/2)+B$12</f>
-        <v>0.4951388889</v>
-      </c>
-      <c r="H5" s="15">
+        <v>0.49513888888888885</v>
+      </c>
+      <c r="H5" s="11">
         <f>((10*60)+53)</f>
         <v>653</v>
       </c>
-      <c r="I5" s="23">
-        <v>91904.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="14">
-        <v>0.020833333333333332</v>
+      <c r="I5" s="16">
+        <v>91904</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="10">
         <v>0.15763888888888888</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="10">
         <v>0.24097222222222223</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="12">
         <f>((3*60)+47)*256</f>
         <v>58112</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((5*60)+47)*256</f>
         <v>88832</v>
       </c>
-      <c r="F2" s="14">
-        <f t="shared" ref="F2:F3" si="1">((C2+B2)/2)-B$12</f>
-        <v>0.1784722222</v>
-      </c>
-      <c r="G2" s="14">
-        <f t="shared" ref="G2:G3" si="2">((C2+B2)/2)+B$12</f>
-        <v>0.2201388889</v>
-      </c>
-      <c r="H2" s="15">
+      <c r="F2" s="10">
+        <f t="shared" ref="F2:F3" si="0">((C2+B2)/2)-B$12</f>
+        <v>0.17847222222222223</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" ref="G2:G3" si="1">((C2+B2)/2)+B$12</f>
+        <v>0.22013888888888891</v>
+      </c>
+      <c r="H2" s="11">
         <f>((4*60)+17)*128</f>
         <v>32896</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
-        <v>0.2548611111111111</v>
-      </c>
-      <c r="C3" s="14">
+      <c r="B3" s="10">
+        <v>0.25486111111111109</v>
+      </c>
+      <c r="C3" s="10">
         <v>0.4777777777777778</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="12">
         <f>((6*60)+7)*256</f>
         <v>93952</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((11*60)+28)*256</f>
         <v>176128</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="10">
+        <f t="shared" si="0"/>
+        <v>0.3454861111111111</v>
+      </c>
+      <c r="G3" s="10">
         <f t="shared" si="1"/>
-        <v>0.3454861111</v>
-      </c>
-      <c r="G3" s="14">
-        <f t="shared" si="2"/>
-        <v>0.3871527778</v>
-      </c>
-      <c r="H3" s="15">
+        <v>0.38715277777777773</v>
+      </c>
+      <c r="H3" s="11">
         <f>((8*60)+17)*128</f>
         <v>63616</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
-        <v>0.5243055555555556</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0.5659722222222222</v>
-      </c>
-      <c r="D4" s="16">
+      <c r="B4" s="10">
+        <v>0.52430555555555558</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D4" s="12">
         <f>((12*60)+35)*256</f>
         <v>193280</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((13*60)+35)*256</f>
         <v>208640</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
-        <v>0.5715277777777777</v>
-      </c>
-      <c r="C5" s="14">
-        <v>0.6131944444444445</v>
-      </c>
-      <c r="D5" s="16">
+      <c r="B5" s="10">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="D5" s="12">
         <f>((13*60)+43)*256</f>
         <v>210688</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((14*60)+43)*256</f>
         <v>226048</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="10">
         <f>((C5+B5)/2)-B$12</f>
-        <v>0.5715277778</v>
-      </c>
-      <c r="G5" s="14">
+        <v>0.57152777777777775</v>
+      </c>
+      <c r="G5" s="10">
         <f>((C5+B5)/2)+B$12</f>
-        <v>0.6131944444</v>
-      </c>
-      <c r="H5" s="15">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="H5" s="11">
         <f>((13*60)+43)*128</f>
         <v>105344</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="14">
-        <v>0.020833333333333332</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.035416666666666666</v>
-      </c>
-      <c r="C2" s="14">
-        <v>0.11875</v>
-      </c>
-      <c r="D2" s="15">
+      <c r="B2" s="10">
+        <v>3.5416666666666666E-2</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.11874999999999999</v>
+      </c>
+      <c r="D2" s="11">
         <f>51*256</f>
         <v>13056</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+51)*256</f>
         <v>43776</v>
       </c>
-      <c r="F2" s="14">
-        <f t="shared" ref="F2:F3" si="1">((C2+B2)/2)-B$12</f>
-        <v>0.05625</v>
-      </c>
-      <c r="G2" s="14">
-        <f t="shared" ref="G2:G3" si="2">((C2+B2)/2)+B$12</f>
-        <v>0.09791666667</v>
-      </c>
-      <c r="H2" s="15">
+      <c r="F2" s="10">
+        <f t="shared" ref="F2:F3" si="0">((C2+B2)/2)-B$12</f>
+        <v>5.6250000000000008E-2</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" ref="G2:G3" si="1">((C2+B2)/2)+B$12</f>
+        <v>9.7916666666666666E-2</v>
+      </c>
+      <c r="H2" s="11">
         <f>((1*60)+21)*256</f>
         <v>20736</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.125</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="10">
         <v>0.38958333333333334</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <f>((3*60)+2)*256</f>
         <v>46592</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((9*60)+21)*256</f>
         <v>143616</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="10">
+        <f t="shared" si="0"/>
+        <v>0.23645833333333335</v>
+      </c>
+      <c r="G3" s="10">
         <f t="shared" si="1"/>
-        <v>0.2364583333</v>
-      </c>
-      <c r="G3" s="14">
-        <f t="shared" si="2"/>
-        <v>0.278125</v>
-      </c>
-      <c r="H3" s="15">
+        <v>0.27812500000000001</v>
+      </c>
+      <c r="H3" s="11">
         <f>((5*60)+40)*256</f>
         <v>87040</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
-        <v>0.3958333333333333</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="10">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C4" s="10">
         <v>0.4375</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <f>((9*60)+30)*256</f>
         <v>145920</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((10*60)+30)*256</f>
         <v>161280</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.44027777777777777</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <v>0.48194444444444445</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <f>((10*60)+34)*256</f>
         <v>162304</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((11*60)+34)*256</f>
         <v>177664</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="10">
         <f>((C5+B5)/2)-B$12</f>
-        <v>0.4402777778</v>
-      </c>
-      <c r="G5" s="14">
+        <v>0.44027777777777782</v>
+      </c>
+      <c r="G5" s="10">
         <f>((C5+B5)/2)+B$12</f>
-        <v>0.4819444444</v>
-      </c>
-      <c r="H5" s="15">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="H5" s="11">
         <f>((10*60)+34)*256</f>
         <v>162304</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="14">
-        <v>0.020833333333333332</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.034722222222222224</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.11805555555555555</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <f>50*256</f>
         <v>12800</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+50)*256</f>
         <v>43520</v>
       </c>
-      <c r="F2" s="14">
-        <f t="shared" ref="F2:F3" si="1">((C2+B2)/2)-B$12</f>
-        <v>0.05555555556</v>
-      </c>
-      <c r="G2" s="14">
-        <f t="shared" ref="G2:G3" si="2">((C2+B2)/2)+B$12</f>
-        <v>0.09722222222</v>
-      </c>
-      <c r="H2" s="15">
+      <c r="F2" s="10">
+        <f t="shared" ref="F2:F3" si="0">((C2+B2)/2)-B$12</f>
+        <v>5.5555555555555566E-2</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" ref="G2:G3" si="1">((C2+B2)/2)+B$12</f>
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="H2" s="11">
         <f>((1*60)+20)*256</f>
         <v>20480</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.125</v>
       </c>
-      <c r="C3" s="14">
-        <v>0.3875</v>
-      </c>
-      <c r="D3" s="15">
+      <c r="C3" s="10">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="D3" s="11">
         <f>((3*60)+2)*256</f>
         <v>46592</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((9*60)+18)*256</f>
         <v>142848</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="10">
+        <f t="shared" si="0"/>
+        <v>0.23541666666666664</v>
+      </c>
+      <c r="G3" s="10">
         <f t="shared" si="1"/>
-        <v>0.2354166667</v>
-      </c>
-      <c r="G3" s="14">
-        <f t="shared" si="2"/>
-        <v>0.2770833333</v>
-      </c>
-      <c r="H3" s="15">
+        <v>0.27708333333333329</v>
+      </c>
+      <c r="H3" s="11">
         <f>((5*60)+39)*256</f>
         <v>86784</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.39444444444444443</v>
       </c>
-      <c r="C4" s="14">
-        <v>0.4361111111111111</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C4" s="10">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="D4" s="11">
         <f>((9*60)+28)*256</f>
         <v>145408</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((10*60)+28)*256</f>
         <v>160768</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.44027777777777777</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <v>0.48194444444444445</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <f>((10*60)+34)*256</f>
         <v>162304</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((11*60)+34)*256</f>
         <v>177664</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="10">
         <f>((C5+B5)/2)-B$12</f>
-        <v>0.4402777778</v>
-      </c>
-      <c r="G5" s="14">
+        <v>0.44027777777777782</v>
+      </c>
+      <c r="G5" s="10">
         <f>((C5+B5)/2)+B$12</f>
-        <v>0.4819444444</v>
-      </c>
-      <c r="H5" s="15">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="H5" s="11">
         <f>((10*60)+34)*256</f>
         <v>162304</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="14">
-        <v>0.020833333333333332</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.034722222222222224</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.11805555555555555</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <f>50*256</f>
         <v>12800</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+50)*256</f>
         <v>43520</v>
       </c>
-      <c r="F2" s="15">
-        <f t="shared" ref="F2:F3" si="1">(E2-D2)/256</f>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F3" si="0">(E2-D2)/256</f>
         <v>120</v>
       </c>
-      <c r="G2" s="14">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="H2" s="14">
-        <v>0.09722222222222222</v>
-      </c>
-      <c r="I2" s="15">
+      <c r="G2" s="10">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="I2" s="11">
         <f>((1*60)+20)*256</f>
         <v>20480</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.12291666666666666</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="10">
         <v>0.23819444444444443</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <f>((2*60)+57)*256</f>
         <v>45312</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((5*60)+43)*256</f>
         <v>87808</v>
       </c>
-      <c r="F3" s="15">
-        <f t="shared" si="1"/>
+      <c r="F3" s="11">
+        <f t="shared" si="0"/>
         <v>166</v>
       </c>
-      <c r="G3" s="14">
-        <v>0.1597222222222222</v>
-      </c>
-      <c r="H3" s="14">
+      <c r="G3" s="10">
+        <v>0.15972222222222221</v>
+      </c>
+      <c r="H3" s="10">
         <v>0.2013888888888889</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="11">
         <f>((3*60)+50)*256</f>
         <v>58880</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.24722222222222223</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="10">
         <v>0.28888888888888886</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <f>((5*60)+56)*256</f>
         <v>91136</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((6*60)+56)*256</f>
         <v>106496</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.28888888888888886</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <v>0.33055555555555555</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <f>((6*60)+56)*256</f>
         <v>106496</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((7*60)+56)*256</f>
         <v>121856</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>(E5-D5)/256</f>
         <v>60</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="10">
         <v>0.28888888888888886</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="10">
         <v>0.33055555555555555</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <f>((6*60)+56)*256</f>
         <v>106496</v>
       </c>
@@ -1524,160 +1512,162 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.03680555555555556</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.6805555555555557E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.12013888888888889</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <f>53*256</f>
         <v>13568</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+53)*256</f>
         <v>44288</v>
       </c>
-      <c r="F2" s="15">
-        <f t="shared" ref="F2:F3" si="1">(E2-D2)/256</f>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F3" si="0">(E2-D2)/256</f>
         <v>120</v>
       </c>
-      <c r="G2" s="14">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="H2" s="14">
-        <v>0.09722222222222222</v>
-      </c>
-      <c r="I2" s="15">
+      <c r="G2" s="10">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="I2" s="11">
         <f>((1*60)+20)*256</f>
         <v>20480</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.13541666666666666</v>
       </c>
-      <c r="C3" s="14">
-        <v>0.2847222222222222</v>
-      </c>
-      <c r="D3" s="15">
+      <c r="C3" s="10">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="D3" s="11">
         <f>((3*60)+15)*256</f>
         <v>49920</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((6*60)+50)*256</f>
         <v>104960</v>
       </c>
-      <c r="F3" s="15">
-        <f t="shared" si="1"/>
+      <c r="F3" s="11">
+        <f t="shared" si="0"/>
         <v>215</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="10">
         <v>0.18958333333333333</v>
       </c>
-      <c r="H3" s="14">
-        <v>0.23125</v>
-      </c>
-      <c r="I3" s="15">
+      <c r="H3" s="10">
+        <v>0.23125000000000001</v>
+      </c>
+      <c r="I3" s="11">
         <f>((4*60)+33)*256</f>
         <v>69888</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.2986111111111111</v>
       </c>
-      <c r="C4" s="14">
-        <v>0.3402777777777778</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C4" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="D4" s="11">
         <f>((7*60)+10)*256</f>
         <v>110080</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((8*60)+10)*256</f>
         <v>125440</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.34375</v>
       </c>
-      <c r="C5" s="14">
-        <v>0.3854166666666667</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C5" s="10">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D5" s="11">
         <f>((8*60)+15)*256</f>
         <v>126720</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((9*60)+15)*256</f>
         <v>142080</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>(E5-D5)/256</f>
         <v>60</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="10">
         <v>0.34375</v>
       </c>
-      <c r="H5" s="14">
-        <v>0.3854166666666667</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="H5" s="10">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="I5" s="11">
         <f>((8*60)+15)*256</f>
         <v>126720</v>
       </c>
@@ -1686,160 +1676,164 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.0375</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.12083333333333333</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <f>54*256</f>
         <v>13824</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+54)*256</f>
         <v>44544</v>
       </c>
-      <c r="F2" s="15">
-        <f t="shared" ref="F2:F3" si="1">(E2-D2)/256</f>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F3" si="0">(E2-D2)/256</f>
         <v>120</v>
       </c>
-      <c r="G2" s="14">
-        <v>0.044444444444444446</v>
-      </c>
-      <c r="H2" s="14">
-        <v>0.08611111111111111</v>
-      </c>
-      <c r="I2" s="15">
+      <c r="G2" s="10">
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>8.611111111111111E-2</v>
+      </c>
+      <c r="I2" s="11">
         <f>((1*60)+4)*256</f>
         <v>16384</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
-        <v>0.1284722222222222</v>
-      </c>
-      <c r="C3" s="14">
+      <c r="B3" s="10">
+        <v>0.12847222222222221</v>
+      </c>
+      <c r="C3" s="10">
         <v>0.24305555555555555</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <f>((3*60)+5)*256</f>
         <v>47360</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((5*60)+50)*256</f>
         <v>89600</v>
       </c>
-      <c r="F3" s="15">
-        <f t="shared" si="1"/>
+      <c r="F3" s="11">
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="10">
         <v>0.14791666666666667</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="10">
         <v>0.18958333333333333</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="11">
         <f>((3*60)+33)*256</f>
         <v>54528</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
-        <v>0.2520833333333333</v>
-      </c>
-      <c r="C4" s="14">
-        <v>0.29375</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="B4" s="10">
+        <v>0.25208333333333333</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="D4" s="11">
         <f>((6*60)+3)*256</f>
         <v>92928</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((7*60)+3)*256</f>
         <v>108288</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.29583333333333334</v>
       </c>
-      <c r="C5" s="14">
-        <v>0.3375</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C5" s="10">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="D5" s="11">
         <f>((7*60)+6)*256</f>
         <v>109056</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((8*60)+6)*256</f>
         <v>124416</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>(E5-D5)/256</f>
         <v>60</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="10">
         <v>0.29583333333333334</v>
       </c>
-      <c r="H5" s="14">
-        <v>0.3375</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="H5" s="10">
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="I5" s="11">
         <f>((7*60)+6)*256</f>
         <v>109056</v>
       </c>
@@ -1848,160 +1842,164 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.034722222222222224</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.11805555555555555</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <f>50*256</f>
         <v>12800</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+50)*256</f>
         <v>43520</v>
       </c>
-      <c r="F2" s="15">
-        <f t="shared" ref="F2:F3" si="1">(E2-D2)/256</f>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F3" si="0">(E2-D2)/256</f>
         <v>120</v>
       </c>
-      <c r="G2" s="14">
-        <v>0.05555555555555555</v>
-      </c>
-      <c r="H2" s="14">
-        <v>0.09722222222222222</v>
-      </c>
-      <c r="I2" s="15">
+      <c r="G2" s="10">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="H2" s="10">
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="I2" s="11">
         <f>((1*60)+20)*256</f>
         <v>20480</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.12638888888888888</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="10">
         <v>0.24097222222222223</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <f>((3*60)+2)*256</f>
         <v>46592</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((5*60)+47)*256</f>
         <v>88832</v>
       </c>
-      <c r="F3" s="15">
-        <f t="shared" si="1"/>
+      <c r="F3" s="11">
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="10">
         <v>0.16319444444444445</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="10">
         <v>0.2048611111111111</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="11">
         <f>((3*60)+55)*256</f>
         <v>60160</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.24791666666666667</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="10">
         <v>0.28958333333333336</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <f>((5*60)+57)*256</f>
         <v>91392</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((6*60)+57)*256</f>
         <v>106752</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
-        <v>0.29375</v>
-      </c>
-      <c r="C5" s="14">
+      <c r="B5" s="10">
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="C5" s="10">
         <v>0.33541666666666664</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <f>((7*60)+3)*256</f>
         <v>108288</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((8*60)+3)*256</f>
         <v>123648</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>(E5-D5)/256</f>
         <v>60</v>
       </c>
-      <c r="G5" s="14">
-        <v>0.29375</v>
-      </c>
-      <c r="H5" s="14">
+      <c r="G5" s="10">
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="H5" s="10">
         <v>0.33541666666666664</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <f>((7*60)+3)*256</f>
         <v>108288</v>
       </c>
@@ -2010,160 +2008,164 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.034722222222222224</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.11805555555555555</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="11">
         <f>50*256</f>
         <v>12800</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+50)*256</f>
         <v>43520</v>
       </c>
-      <c r="F2" s="15">
-        <f t="shared" ref="F2:F3" si="1">(E2-D2)/256</f>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F3" si="0">(E2-D2)/256</f>
         <v>120</v>
       </c>
-      <c r="G2" s="14">
-        <v>0.07291666666666667</v>
-      </c>
-      <c r="H2" s="14">
+      <c r="G2" s="10">
+        <v>7.2916666666666671E-2</v>
+      </c>
+      <c r="H2" s="10">
         <v>0.11458333333333333</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="11">
         <f>((1*60)+45)*256</f>
         <v>26880</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
-        <v>0.1284722222222222</v>
-      </c>
-      <c r="C3" s="14">
+      <c r="B3" s="10">
+        <v>0.12847222222222221</v>
+      </c>
+      <c r="C3" s="10">
         <v>0.29305555555555557</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <f>((3*60)+5)*256</f>
         <v>47360</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((7*60)+2)*256</f>
         <v>108032</v>
       </c>
-      <c r="F3" s="15">
-        <f t="shared" si="1"/>
+      <c r="F3" s="11">
+        <f t="shared" si="0"/>
         <v>237</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="10">
         <v>0.19027777777777777</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="10">
         <v>0.23194444444444445</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="11">
         <f>((4*60)+34)*256</f>
         <v>70144</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.2986111111111111</v>
       </c>
-      <c r="C4" s="14">
-        <v>0.3402777777777778</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C4" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="D4" s="11">
         <f>((5*60)+10)*256</f>
         <v>79360</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((8*60)+10)*256</f>
         <v>125440</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.34444444444444444</v>
       </c>
-      <c r="C5" s="14">
-        <v>0.3861111111111111</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C5" s="10">
+        <v>0.38611111111111113</v>
+      </c>
+      <c r="D5" s="11">
         <f>((7*60)+16)*256</f>
         <v>111616</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((8*60)+16)*256</f>
         <v>126976</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>(E5-D5)/256</f>
         <v>60</v>
       </c>
-      <c r="G5" s="14">
-        <v>0.3402777777777778</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0.3819444444444444</v>
-      </c>
-      <c r="I5" s="15">
+      <c r="G5" s="10">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="I5" s="11">
         <f>((8*60)+10)*256</f>
         <v>125440</v>
       </c>
@@ -2172,160 +2174,164 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="10">
         <v>0.11319444444444444</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="10">
         <v>0.19652777777777777</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="12">
         <f>((2*60)+43)*256</f>
         <v>41728</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((4*60)+43)*256</f>
         <v>72448</v>
       </c>
-      <c r="F2" s="15">
-        <f t="shared" ref="F2:F3" si="1">(E2-D2)/256</f>
+      <c r="F2" s="11">
+        <f t="shared" ref="F2:F3" si="0">(E2-D2)/256</f>
         <v>120</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="10">
         <v>0.13402777777777777</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="10">
         <v>0.17569444444444443</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="11">
         <f>((3*60)+13)*256</f>
         <v>49408</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.2013888888888889</v>
       </c>
-      <c r="C3" s="14">
-        <v>0.3736111111111111</v>
-      </c>
-      <c r="D3" s="15">
+      <c r="C3" s="10">
+        <v>0.37361111111111112</v>
+      </c>
+      <c r="D3" s="11">
         <f>((4*60)+50)*256</f>
         <v>74240</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((8*60)+58)*256</f>
         <v>137728</v>
       </c>
-      <c r="F3" s="15">
-        <f t="shared" si="1"/>
+      <c r="F3" s="11">
+        <f t="shared" si="0"/>
         <v>248</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="10">
         <v>0.26666666666666666</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="10">
         <v>0.30833333333333335</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="11">
         <f>((6*60)+24)*256</f>
         <v>98304</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.38958333333333334</v>
       </c>
-      <c r="C4" s="14">
-        <v>0.43125</v>
-      </c>
-      <c r="D4" s="15">
+      <c r="C4" s="10">
+        <v>0.43125000000000002</v>
+      </c>
+      <c r="D4" s="11">
         <f>((9*60)+21)*256</f>
         <v>143616</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((10*60)+21)*256</f>
         <v>158976</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.43819444444444444</v>
       </c>
-      <c r="C5" s="14">
-        <v>0.4798611111111111</v>
-      </c>
-      <c r="D5" s="15">
+      <c r="C5" s="10">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="D5" s="11">
         <f>((10*60)+31)*256</f>
         <v>161536</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((11*60)+31)*256</f>
         <v>176896</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="11">
         <f>(E5-D5)/256</f>
         <v>60</v>
       </c>
-      <c r="G5" s="14">
-        <v>0.43125</v>
-      </c>
-      <c r="H5" s="14">
+      <c r="G5" s="10">
+        <v>0.43125000000000002</v>
+      </c>
+      <c r="H5" s="10">
         <v>0.47291666666666665</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <f>((10*60)+21)*256</f>
         <v>158976</v>
       </c>
@@ -2334,340 +2340,348 @@
   <mergeCells count="1">
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="19">
-        <v>0.03958333333333333</v>
-      </c>
-      <c r="C2" s="19">
+      <c r="B2" s="14">
+        <v>3.9583333333333331E-2</v>
+      </c>
+      <c r="C2" s="14">
         <v>0.12291666666666666</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="8">
         <f>57*256</f>
         <v>14592</v>
       </c>
-      <c r="E2" s="20">
+      <c r="E2" s="8">
         <f>((2*60)+57)*256</f>
         <v>45312</v>
       </c>
-      <c r="F2" s="19">
-        <f t="shared" ref="F2:F3" si="1">((C2+B2)/2)-B$12</f>
-        <v>0.06041666667</v>
-      </c>
-      <c r="G2" s="19">
-        <f t="shared" ref="G2:G3" si="2">((C2+B2)/2)+B$12</f>
-        <v>0.1020833333</v>
-      </c>
-      <c r="H2" s="20">
+      <c r="F2" s="14">
+        <f t="shared" ref="F2:F3" si="0">((C2+B2)/2)-B$12</f>
+        <v>6.041666666666666E-2</v>
+      </c>
+      <c r="G2" s="14">
+        <f t="shared" ref="G2:G3" si="1">((C2+B2)/2)+B$12</f>
+        <v>0.10208333333333332</v>
+      </c>
+      <c r="H2" s="8">
         <f>((1*60)+27)</f>
         <v>87</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="14">
         <v>0.14027777777777778</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="14">
         <v>0.3125</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="8">
         <f>((3*60)+22)*256</f>
         <v>51712</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="8">
         <f>((7*60)+30)*256</f>
         <v>115200</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="14">
+        <f t="shared" si="0"/>
+        <v>0.20555555555555555</v>
+      </c>
+      <c r="G3" s="14">
         <f t="shared" si="1"/>
-        <v>0.2055555556</v>
-      </c>
-      <c r="G3" s="19">
-        <f t="shared" si="2"/>
-        <v>0.2472222222</v>
-      </c>
-      <c r="H3" s="20">
+        <v>0.24722222222222223</v>
+      </c>
+      <c r="H3" s="8">
         <f>((4*60)+56)</f>
         <v>296</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="19">
-        <v>0.3194444444444444</v>
-      </c>
-      <c r="C4" s="19">
+      <c r="B4" s="14">
+        <v>0.31944444444444442</v>
+      </c>
+      <c r="C4" s="14">
         <v>0.3611111111111111</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="8">
         <f>((7*60)+40)*256</f>
         <v>117760</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="8">
         <f>((8*60)+40)*256</f>
         <v>133120</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="14">
         <v>0.3659722222222222</v>
       </c>
-      <c r="C5" s="19">
-        <v>0.4076388888888889</v>
-      </c>
-      <c r="D5" s="20">
+      <c r="C5" s="14">
+        <v>0.40763888888888888</v>
+      </c>
+      <c r="D5" s="8">
         <f>((8*60)+47)*256</f>
         <v>134912</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="8">
         <f>((9*60)+47)*256</f>
         <v>150272</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="14">
         <f>((C5+B5)/2)-B$12</f>
-        <v>0.3659722222</v>
-      </c>
-      <c r="G5" s="19">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="G5" s="14">
         <f>((C5+B5)/2)+B$12</f>
-        <v>0.4076388889</v>
-      </c>
-      <c r="H5" s="20">
+        <v>0.40763888888888883</v>
+      </c>
+      <c r="H5" s="8">
         <f>((8*60)+47)</f>
         <v>527</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="22">
-        <v>0.020833333333333332</v>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="15">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="14">
-        <v>0.03611111111111111</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="10">
+        <v>3.6111111111111108E-2</v>
+      </c>
+      <c r="C2" s="10">
         <v>0.11944444444444445</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="12">
         <f>(52)*256</f>
         <v>13312</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="11">
         <f>((2*60)+52)*256</f>
         <v>44032</v>
       </c>
-      <c r="F2" s="14">
-        <f t="shared" ref="F2:F3" si="1">((C2+B2)/2)-B$12</f>
-        <v>0.05694444444</v>
-      </c>
-      <c r="G2" s="14">
-        <f t="shared" ref="G2:G3" si="2">((C2+B2)/2)+B$12</f>
-        <v>0.09861111111</v>
-      </c>
-      <c r="H2" s="15">
+      <c r="F2" s="10">
+        <f t="shared" ref="F2:F3" si="0">((C2+B2)/2)-B$12</f>
+        <v>5.694444444444445E-2</v>
+      </c>
+      <c r="G2" s="10">
+        <f t="shared" ref="G2:G3" si="1">((C2+B2)/2)+B$12</f>
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="H2" s="11">
         <f>((1*60)+22)</f>
         <v>82</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <v>0.13819444444444445</v>
       </c>
-      <c r="C3" s="14">
-        <v>0.30625</v>
-      </c>
-      <c r="D3" s="16">
+      <c r="C3" s="10">
+        <v>0.30625000000000002</v>
+      </c>
+      <c r="D3" s="12">
         <f>((3*60)+19)*256</f>
         <v>50944</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="11">
         <f>((7*60)+21)*256</f>
         <v>112896</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="10">
+        <f t="shared" si="0"/>
+        <v>0.2013888888888889</v>
+      </c>
+      <c r="G3" s="10">
         <f t="shared" si="1"/>
-        <v>0.2013888889</v>
-      </c>
-      <c r="G3" s="14">
-        <f t="shared" si="2"/>
-        <v>0.2430555556</v>
-      </c>
-      <c r="H3" s="15">
+        <v>0.24305555555555558</v>
+      </c>
+      <c r="H3" s="11">
         <f>((4*60)+50)</f>
         <v>290</v>
       </c>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="13" t="s">
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="10">
         <v>0.31180555555555556</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="10">
         <v>0.35347222222222224</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="12">
         <f>((7*60)+29)*256</f>
         <v>114944</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>((8*60)+29)*256</f>
         <v>130304</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="10">
         <v>0.35833333333333334</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="10">
         <v>0.4</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="12">
         <f>((8*60)+36)*256</f>
         <v>132096</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>((9*60)+36)*256</f>
         <v>147456</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="10">
         <f>((C5+B5)/2)-B$12</f>
-        <v>0.3583333333</v>
-      </c>
-      <c r="G5" s="14">
+        <v>0.35833333333333334</v>
+      </c>
+      <c r="G5" s="10">
         <f>((C5+B5)/2)+B$12</f>
-        <v>0.4</v>
-      </c>
-      <c r="H5" s="15">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="H5" s="11">
         <f>((8*60)+36)</f>
         <v>516</v>
       </c>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="14">
-        <v>0.020833333333333332</v>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>